<commit_message>
révisions de l'article et nouveaux graphiques
</commit_message>
<xml_diff>
--- a/cas types smic_calculs.xlsx
+++ b/cas types smic_calculs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20416"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20417"/>
   <workbookPr codeName="ThisWorkbook" checkCompatibility="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/FC63792E2F244A79/Documents/GitHub/PB_GainEmploi/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mpucci\OneDrive\Documents\GitHub\PB_GainEmploi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="8_{88ADA55B-E4F3-49D2-B497-9395CD85FE86}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{13B6D672-5E15-4CC0-A9CE-1531311C0E8E}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="8_{88ADA55B-E4F3-49D2-B497-9395CD85FE86}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{92FF660D-895E-4D45-96CF-8C9A16C9AA3D}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="4" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -493,7 +493,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1667" uniqueCount="565">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1668" uniqueCount="566">
   <si>
     <t>RSA forfaitaire</t>
   </si>
@@ -2270,6 +2270,9 @@
   </si>
   <si>
     <t>nviesspa/seuil</t>
+  </si>
+  <si>
+    <t>TEG</t>
   </si>
 </sst>
 </file>
@@ -3720,7 +3723,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="50" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="517">
+  <cellXfs count="516">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="24" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="24" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -4865,14 +4868,50 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" xfId="37" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" indent="3"/>
-    </xf>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="40" fillId="43" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="40" fillId="43" borderId="0" xfId="37" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="43" borderId="0" xfId="37" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="43" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="28" fillId="27" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="28" fillId="27" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="28" fillId="27" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="28" fillId="27" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="28" fillId="27" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="28" fillId="27" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="28" fillId="27" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="28" fillId="27" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="28" fillId="27" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -4935,45 +4974,6 @@
     </xf>
     <xf numFmtId="10" fontId="28" fillId="27" borderId="30" xfId="37" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="28" fillId="27" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="28" fillId="27" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="28" fillId="27" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="28" fillId="27" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="28" fillId="27" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="28" fillId="27" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="28" fillId="27" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="28" fillId="27" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="28" fillId="27" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="34" fillId="37" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -5447,10 +5447,10 @@
       <c r="D3" s="97">
         <v>1353.07</v>
       </c>
-      <c r="E3" s="501" t="s">
+      <c r="E3" s="479" t="s">
         <v>471</v>
       </c>
-      <c r="F3" s="501"/>
+      <c r="F3" s="479"/>
     </row>
     <row r="4" spans="1:6" s="12" customFormat="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="17" t="s">
@@ -5464,10 +5464,10 @@
       <c r="D4" s="97">
         <v>1269.02</v>
       </c>
-      <c r="E4" s="501" t="s">
+      <c r="E4" s="479" t="s">
         <v>472</v>
       </c>
-      <c r="F4" s="501"/>
+      <c r="F4" s="479"/>
     </row>
     <row r="5" spans="1:6" s="12" customFormat="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="17" t="s">
@@ -5481,10 +5481,10 @@
       <c r="D5" s="388">
         <v>1107.348</v>
       </c>
-      <c r="E5" s="501" t="s">
+      <c r="E5" s="479" t="s">
         <v>446</v>
       </c>
-      <c r="F5" s="501"/>
+      <c r="F5" s="479"/>
     </row>
     <row r="6" spans="1:6" s="12" customFormat="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="17" t="s">
@@ -5498,10 +5498,10 @@
         <f>smic/smic_2012</f>
         <v>1.263107893814772</v>
       </c>
-      <c r="E6" s="513" t="s">
+      <c r="E6" s="491" t="s">
         <v>473</v>
       </c>
-      <c r="F6" s="513"/>
+      <c r="F6" s="491"/>
     </row>
     <row r="7" spans="1:6" s="12" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A7" s="13"/>
@@ -5633,10 +5633,10 @@
         <f>0.9*((1+assiette_csgcrds*(crds+tx_csgimp)/(1-tx_cotsal)))*12</f>
         <v>11.197672525200311</v>
       </c>
-      <c r="D18" s="511" t="s">
+      <c r="D18" s="489" t="s">
         <v>201</v>
       </c>
-      <c r="E18" s="512"/>
+      <c r="E18" s="490"/>
       <c r="F18" s="99">
         <v>5.0000000000000001E-3</v>
       </c>
@@ -5667,10 +5667,10 @@
       <c r="B21" s="395">
         <v>43992</v>
       </c>
-      <c r="D21" s="511" t="s">
+      <c r="D21" s="489" t="s">
         <v>509</v>
       </c>
-      <c r="E21" s="512"/>
+      <c r="E21" s="490"/>
       <c r="F21" s="99">
         <v>1.1299999999999999</v>
       </c>
@@ -5682,10 +5682,10 @@
       <c r="B22" s="395">
         <v>41136</v>
       </c>
-      <c r="D22" s="511" t="s">
+      <c r="D22" s="489" t="s">
         <v>508</v>
       </c>
-      <c r="E22" s="512"/>
+      <c r="E22" s="490"/>
       <c r="F22" s="99">
         <f>F20*F21</f>
         <v>1308.54</v>
@@ -7006,11 +7006,11 @@
       <c r="D125" s="62"/>
       <c r="E125" s="63"/>
       <c r="F125" s="64"/>
-      <c r="G125" s="502">
+      <c r="G125" s="480">
         <v>58.08</v>
       </c>
-      <c r="H125" s="503"/>
-      <c r="I125" s="504"/>
+      <c r="H125" s="481"/>
+      <c r="I125" s="482"/>
     </row>
     <row r="126" spans="1:9" s="12" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A126" s="65" t="s">
@@ -7021,11 +7021,11 @@
       <c r="D126" s="66"/>
       <c r="E126" s="67"/>
       <c r="F126" s="68"/>
-      <c r="G126" s="505">
+      <c r="G126" s="483">
         <v>71.25</v>
       </c>
-      <c r="H126" s="506"/>
-      <c r="I126" s="507"/>
+      <c r="H126" s="484"/>
+      <c r="I126" s="485"/>
     </row>
     <row r="127" spans="1:9" s="12" customFormat="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A127" s="69" t="s">
@@ -7036,11 +7036,11 @@
       <c r="D127" s="70"/>
       <c r="E127" s="71"/>
       <c r="F127" s="72"/>
-      <c r="G127" s="508">
+      <c r="G127" s="486">
         <v>13.17</v>
       </c>
-      <c r="H127" s="509"/>
-      <c r="I127" s="510"/>
+      <c r="H127" s="487"/>
+      <c r="I127" s="488"/>
     </row>
     <row r="128" spans="1:9" s="12" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A128" s="61" t="s">
@@ -7186,11 +7186,11 @@
       <c r="D137" s="74"/>
       <c r="E137" s="75"/>
       <c r="F137" s="167"/>
-      <c r="G137" s="488">
+      <c r="G137" s="500">
         <v>37.909999999999997</v>
       </c>
-      <c r="H137" s="488"/>
-      <c r="I137" s="488"/>
+      <c r="H137" s="500"/>
+      <c r="I137" s="500"/>
     </row>
     <row r="138" spans="1:9" s="12" customFormat="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A138" s="73" t="s">
@@ -7201,11 +7201,11 @@
       <c r="D138" s="74"/>
       <c r="E138" s="75"/>
       <c r="F138" s="76"/>
-      <c r="G138" s="492">
+      <c r="G138" s="504">
         <v>8.5000000000000006E-2</v>
       </c>
-      <c r="H138" s="493"/>
-      <c r="I138" s="494"/>
+      <c r="H138" s="505"/>
+      <c r="I138" s="506"/>
     </row>
     <row r="139" spans="1:9" s="12" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A139" s="61" t="s">
@@ -7216,11 +7216,11 @@
       <c r="D139" s="62"/>
       <c r="E139" s="63"/>
       <c r="F139" s="64"/>
-      <c r="G139" s="495">
+      <c r="G139" s="507">
         <v>2.8299999999999999E-2</v>
       </c>
-      <c r="H139" s="496"/>
-      <c r="I139" s="497"/>
+      <c r="H139" s="508"/>
+      <c r="I139" s="509"/>
     </row>
     <row r="140" spans="1:9" s="12" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A140" s="65" t="s">
@@ -7231,11 +7231,11 @@
       <c r="D140" s="66"/>
       <c r="E140" s="67"/>
       <c r="F140" s="68"/>
-      <c r="G140" s="489">
+      <c r="G140" s="501">
         <v>3.15E-2</v>
       </c>
-      <c r="H140" s="490"/>
-      <c r="I140" s="491"/>
+      <c r="H140" s="502"/>
+      <c r="I140" s="503"/>
     </row>
     <row r="141" spans="1:9" s="12" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A141" s="65" t="s">
@@ -7246,11 +7246,11 @@
       <c r="D141" s="66"/>
       <c r="E141" s="67"/>
       <c r="F141" s="68"/>
-      <c r="G141" s="489">
+      <c r="G141" s="501">
         <v>2.7E-2</v>
       </c>
-      <c r="H141" s="490"/>
-      <c r="I141" s="491"/>
+      <c r="H141" s="502"/>
+      <c r="I141" s="503"/>
     </row>
     <row r="142" spans="1:9" s="12" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A142" s="65" t="s">
@@ -7261,11 +7261,11 @@
       <c r="D142" s="66"/>
       <c r="E142" s="67"/>
       <c r="F142" s="68"/>
-      <c r="G142" s="489">
+      <c r="G142" s="501">
         <v>2.3800000000000002E-2</v>
       </c>
-      <c r="H142" s="490"/>
-      <c r="I142" s="491"/>
+      <c r="H142" s="502"/>
+      <c r="I142" s="503"/>
     </row>
     <row r="143" spans="1:9" s="12" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A143" s="65" t="s">
@@ -7276,11 +7276,11 @@
       <c r="D143" s="66"/>
       <c r="E143" s="67"/>
       <c r="F143" s="68"/>
-      <c r="G143" s="489">
+      <c r="G143" s="501">
         <v>2.01E-2</v>
       </c>
-      <c r="H143" s="490"/>
-      <c r="I143" s="491"/>
+      <c r="H143" s="502"/>
+      <c r="I143" s="503"/>
     </row>
     <row r="144" spans="1:9" s="12" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A144" s="65" t="s">
@@ -7291,11 +7291,11 @@
       <c r="D144" s="66"/>
       <c r="E144" s="67"/>
       <c r="F144" s="68"/>
-      <c r="G144" s="489">
+      <c r="G144" s="501">
         <v>1.8499999999999999E-2</v>
       </c>
-      <c r="H144" s="490"/>
-      <c r="I144" s="491"/>
+      <c r="H144" s="502"/>
+      <c r="I144" s="503"/>
     </row>
     <row r="145" spans="1:9" s="12" customFormat="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A145" s="69" t="s">
@@ -7306,11 +7306,11 @@
       <c r="D145" s="70"/>
       <c r="E145" s="71"/>
       <c r="F145" s="72"/>
-      <c r="G145" s="498">
+      <c r="G145" s="510">
         <v>-5.9999999999999995E-4</v>
       </c>
-      <c r="H145" s="499"/>
-      <c r="I145" s="500"/>
+      <c r="H145" s="511"/>
+      <c r="I145" s="512"/>
     </row>
     <row r="146" spans="1:9" s="12" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A146" s="61" t="s">
@@ -8122,12 +8122,12 @@
       <c r="B220" s="144" t="s">
         <v>275</v>
       </c>
-      <c r="C220" s="482" t="s">
+      <c r="C220" s="494" t="s">
         <v>276</v>
       </c>
-      <c r="D220" s="483"/>
-      <c r="E220" s="483"/>
-      <c r="F220" s="484"/>
+      <c r="D220" s="495"/>
+      <c r="E220" s="495"/>
+      <c r="F220" s="496"/>
     </row>
     <row r="221" spans="1:6" s="25" customFormat="1" ht="15.5" x14ac:dyDescent="0.25">
       <c r="A221" s="134">
@@ -8196,10 +8196,10 @@
       <c r="B226" s="170">
         <v>8.64</v>
       </c>
-      <c r="C226" s="485"/>
-      <c r="D226" s="486"/>
-      <c r="E226" s="486"/>
-      <c r="F226" s="487"/>
+      <c r="C226" s="497"/>
+      <c r="D226" s="498"/>
+      <c r="E226" s="498"/>
+      <c r="F226" s="499"/>
     </row>
     <row r="227" spans="1:6" s="25" customFormat="1" ht="15.5" x14ac:dyDescent="0.25">
       <c r="A227" s="134" t="s">
@@ -8208,10 +8208,10 @@
       <c r="B227" s="170">
         <v>5</v>
       </c>
-      <c r="C227" s="485"/>
-      <c r="D227" s="486"/>
-      <c r="E227" s="486"/>
-      <c r="F227" s="487"/>
+      <c r="C227" s="497"/>
+      <c r="D227" s="498"/>
+      <c r="E227" s="498"/>
+      <c r="F227" s="499"/>
     </row>
     <row r="228" spans="1:6" s="25" customFormat="1" ht="15.5" x14ac:dyDescent="0.25">
       <c r="A228" s="134" t="s">
@@ -8582,10 +8582,10 @@
       <c r="G262" s="203">
         <v>7190</v>
       </c>
-      <c r="H262" s="480" t="s">
+      <c r="H262" s="492" t="s">
         <v>330</v>
       </c>
-      <c r="I262" s="481"/>
+      <c r="I262" s="493"/>
     </row>
     <row r="263" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A263" s="181">
@@ -8609,8 +8609,8 @@
       <c r="G263" s="203">
         <v>8829</v>
       </c>
-      <c r="H263" s="480"/>
-      <c r="I263" s="481"/>
+      <c r="H263" s="492"/>
+      <c r="I263" s="493"/>
     </row>
     <row r="264" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A264" s="180">
@@ -10160,16 +10160,6 @@
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <mergeCells count="23">
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="G125:I125"/>
-    <mergeCell ref="G126:I126"/>
-    <mergeCell ref="G127:I127"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="D22:E22"/>
     <mergeCell ref="H262:I263"/>
     <mergeCell ref="C220:F220"/>
     <mergeCell ref="C226:F226"/>
@@ -10183,6 +10173,16 @@
     <mergeCell ref="G142:I142"/>
     <mergeCell ref="G140:I140"/>
     <mergeCell ref="G141:I141"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="G125:I125"/>
+    <mergeCell ref="G126:I126"/>
+    <mergeCell ref="G127:I127"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="D22:E22"/>
   </mergeCells>
   <pageMargins left="0.78740157499999996" right="0.78740157499999996" top="0.984251969" bottom="0.984251969" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" scale="64" fitToHeight="8" orientation="portrait" r:id="rId1"/>
@@ -10553,7 +10553,7 @@
       <c r="A40" s="341" t="s">
         <v>206</v>
       </c>
-      <c r="B40" s="514" t="s">
+      <c r="B40" s="513" t="s">
         <v>389</v>
       </c>
       <c r="C40" s="342">
@@ -10565,7 +10565,7 @@
       <c r="A41" s="343" t="s">
         <v>207</v>
       </c>
-      <c r="B41" s="515"/>
+      <c r="B41" s="514"/>
       <c r="C41" s="344">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -12727,30 +12727,30 @@
         <v>387</v>
       </c>
       <c r="B2" s="356"/>
-      <c r="C2" s="516" t="s">
+      <c r="C2" s="515" t="s">
         <v>531</v>
       </c>
-      <c r="D2" s="516"/>
-      <c r="E2" s="516"/>
-      <c r="F2" s="516"/>
-      <c r="H2" s="516" t="s">
+      <c r="D2" s="515"/>
+      <c r="E2" s="515"/>
+      <c r="F2" s="515"/>
+      <c r="H2" s="515" t="s">
         <v>532</v>
       </c>
-      <c r="I2" s="516"/>
-      <c r="J2" s="516"/>
-      <c r="K2" s="516"/>
-      <c r="M2" s="516" t="s">
+      <c r="I2" s="515"/>
+      <c r="J2" s="515"/>
+      <c r="K2" s="515"/>
+      <c r="M2" s="515" t="s">
         <v>533</v>
       </c>
-      <c r="N2" s="516"/>
-      <c r="O2" s="516"/>
-      <c r="P2" s="516"/>
-      <c r="R2" s="516" t="s">
+      <c r="N2" s="515"/>
+      <c r="O2" s="515"/>
+      <c r="P2" s="515"/>
+      <c r="R2" s="515" t="s">
         <v>537</v>
       </c>
-      <c r="S2" s="516"/>
-      <c r="T2" s="516"/>
-      <c r="U2" s="516"/>
+      <c r="S2" s="515"/>
+      <c r="T2" s="515"/>
+      <c r="U2" s="515"/>
     </row>
     <row r="3" spans="1:21" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
@@ -14526,7 +14526,7 @@
       <c r="A40" s="341" t="s">
         <v>206</v>
       </c>
-      <c r="B40" s="514" t="s">
+      <c r="B40" s="513" t="s">
         <v>389</v>
       </c>
       <c r="C40" s="342">
@@ -14598,7 +14598,7 @@
       <c r="A41" s="343" t="s">
         <v>207</v>
       </c>
-      <c r="B41" s="515"/>
+      <c r="B41" s="514"/>
       <c r="C41" s="344">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -29241,30 +29241,30 @@
         <v>387</v>
       </c>
       <c r="B2" s="356"/>
-      <c r="C2" s="516" t="s">
+      <c r="C2" s="515" t="s">
         <v>534</v>
       </c>
-      <c r="D2" s="516"/>
-      <c r="E2" s="516"/>
-      <c r="F2" s="516"/>
-      <c r="H2" s="516" t="s">
+      <c r="D2" s="515"/>
+      <c r="E2" s="515"/>
+      <c r="F2" s="515"/>
+      <c r="H2" s="515" t="s">
         <v>535</v>
       </c>
-      <c r="I2" s="516"/>
-      <c r="J2" s="516"/>
-      <c r="K2" s="516"/>
-      <c r="M2" s="516" t="s">
+      <c r="I2" s="515"/>
+      <c r="J2" s="515"/>
+      <c r="K2" s="515"/>
+      <c r="M2" s="515" t="s">
         <v>536</v>
       </c>
-      <c r="N2" s="516"/>
-      <c r="O2" s="516"/>
-      <c r="P2" s="516"/>
-      <c r="R2" s="516" t="s">
+      <c r="N2" s="515"/>
+      <c r="O2" s="515"/>
+      <c r="P2" s="515"/>
+      <c r="R2" s="515" t="s">
         <v>538</v>
       </c>
-      <c r="S2" s="516"/>
-      <c r="T2" s="516"/>
-      <c r="U2" s="516"/>
+      <c r="S2" s="515"/>
+      <c r="T2" s="515"/>
+      <c r="U2" s="515"/>
     </row>
     <row r="3" spans="1:21" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
@@ -31040,7 +31040,7 @@
       <c r="A40" s="341" t="s">
         <v>206</v>
       </c>
-      <c r="B40" s="514" t="s">
+      <c r="B40" s="513" t="s">
         <v>389</v>
       </c>
       <c r="C40" s="342">
@@ -31112,7 +31112,7 @@
       <c r="A41" s="343" t="s">
         <v>207</v>
       </c>
-      <c r="B41" s="515"/>
+      <c r="B41" s="514"/>
       <c r="C41" s="344">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -45731,10 +45731,10 @@
   <dimension ref="A1:U81"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="T52" sqref="T52:T64"/>
+      <selection pane="bottomRight" activeCell="Q3" sqref="Q3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -45806,8 +45806,11 @@
       <c r="T1" t="s">
         <v>564</v>
       </c>
-    </row>
-    <row r="2" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U1" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" s="461" t="s">
         <v>11</v>
       </c>
@@ -45857,17 +45860,18 @@
         <v>1309</v>
       </c>
       <c r="Q2" s="465">
-        <v>0.65042593582887698</v>
+        <f>M2/1312</f>
+        <v>0.64893868140243893</v>
       </c>
       <c r="R2" s="469">
         <v>0.34957406417112302</v>
       </c>
       <c r="T2" s="465">
         <f>(L2-J2)*Q2/L2</f>
-        <v>0.65042593582887698</v>
-      </c>
-    </row>
-    <row r="3" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+        <v>0.64893868140243893</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" s="461" t="s">
         <v>11</v>
       </c>
@@ -45917,7 +45921,8 @@
         <v>1309</v>
       </c>
       <c r="Q3" s="465">
-        <v>0.90953772200460814</v>
+        <f t="shared" ref="Q3:Q4" si="0">M3/1312</f>
+        <v>0.90745798635978048</v>
       </c>
       <c r="R3" s="469">
         <v>9.046227799539186E-2</v>
@@ -45927,11 +45932,11 @@
         <v>0.48498938743695158</v>
       </c>
       <c r="T3" s="465">
-        <f t="shared" ref="T3:T66" si="0">(L3-J3)*Q3/L3</f>
-        <v>0.70037648403669361</v>
-      </c>
-    </row>
-    <row r="4" spans="1:21" s="89" customFormat="1" ht="13" hidden="1" x14ac:dyDescent="0.3">
+        <f t="shared" ref="T3:T66" si="1">(L3-J3)*Q3/L3</f>
+        <v>0.69877501341770731</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" s="89" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A4" s="268" t="s">
         <v>11</v>
       </c>
@@ -45980,8 +45985,9 @@
       <c r="P4" s="268">
         <v>1309</v>
       </c>
-      <c r="Q4" s="471">
-        <v>1.2648856875477463</v>
+      <c r="Q4" s="465">
+        <f t="shared" si="0"/>
+        <v>1.261993418445122</v>
       </c>
       <c r="R4" s="472" t="s">
         <v>563</v>
@@ -45991,10 +45997,10 @@
         <v>0.57505384642882684</v>
       </c>
       <c r="T4" s="465">
-        <f t="shared" si="0"/>
-        <v>1.0685255920550039</v>
-      </c>
-      <c r="U4" s="475"/>
+        <f t="shared" si="1"/>
+        <v>1.0660823170731708</v>
+      </c>
+      <c r="U4" s="474"/>
     </row>
     <row r="5" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="461" t="s">
@@ -46056,11 +46062,11 @@
         <v>0.55502856893018582</v>
       </c>
       <c r="T5" s="465">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.5400192811642295</v>
       </c>
     </row>
-    <row r="6" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" s="461" t="s">
         <v>11</v>
       </c>
@@ -46110,17 +46116,18 @@
         <v>1309</v>
       </c>
       <c r="Q6" s="465">
-        <v>0.76436001422694955</v>
+        <f t="shared" ref="Q6:Q8" si="2">M6/1312</f>
+        <v>0.76261223980417447</v>
       </c>
       <c r="R6" s="469">
         <v>0.23563998577305045</v>
       </c>
       <c r="T6" s="465">
-        <f t="shared" si="0"/>
-        <v>0.76436001422694955</v>
-      </c>
-    </row>
-    <row r="7" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>0.76261223980417447</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" s="461" t="s">
         <v>11</v>
       </c>
@@ -46170,7 +46177,8 @@
         <v>1309</v>
       </c>
       <c r="Q7" s="465">
-        <v>1.0041723245636716</v>
+        <f t="shared" si="2"/>
+        <v>1.001876198821529</v>
       </c>
       <c r="R7" s="469" t="s">
         <v>563</v>
@@ -46180,11 +46188,11 @@
         <v>0.58352557160220164</v>
       </c>
       <c r="T7" s="465">
-        <f t="shared" si="0"/>
-        <v>0.76630183710994881</v>
-      </c>
-    </row>
-    <row r="8" spans="1:21" s="89" customFormat="1" ht="13" hidden="1" x14ac:dyDescent="0.3">
+        <f t="shared" si="1"/>
+        <v>0.76454962254338632</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" s="89" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A8" s="268" t="s">
         <v>11</v>
       </c>
@@ -46233,8 +46241,9 @@
       <c r="P8" s="268">
         <v>1309</v>
       </c>
-      <c r="Q8" s="471">
-        <v>1.2511046483427599</v>
+      <c r="Q8" s="465">
+        <f t="shared" si="2"/>
+        <v>1.248243890762708</v>
       </c>
       <c r="R8" s="472" t="s">
         <v>563</v>
@@ -46244,8 +46253,8 @@
         <v>0.59218799161712632</v>
       </c>
       <c r="T8" s="465">
-        <f t="shared" si="0"/>
-        <v>1.0667681078244546</v>
+        <f t="shared" si="1"/>
+        <v>1.0643288514803442</v>
       </c>
     </row>
     <row r="9" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
@@ -46308,11 +46317,11 @@
         <v>0.5644077202640545</v>
       </c>
       <c r="T9" s="465">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.3479933514779336</v>
       </c>
     </row>
-    <row r="10" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" s="461" t="s">
         <v>11</v>
       </c>
@@ -46362,17 +46371,18 @@
         <v>1309</v>
       </c>
       <c r="Q10" s="465">
-        <v>0.78438132238349889</v>
+        <f t="shared" ref="Q10:Q12" si="3">M10/1312</f>
+        <v>0.78258776753048787</v>
       </c>
       <c r="R10" s="469">
         <v>0.21561867761650111</v>
       </c>
       <c r="T10" s="465">
-        <f t="shared" si="0"/>
-        <v>0.78438132238349889</v>
-      </c>
-    </row>
-    <row r="11" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>0.78258776753048787</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" s="461" t="s">
         <v>11</v>
       </c>
@@ -46422,7 +46432,8 @@
         <v>1309</v>
       </c>
       <c r="Q11" s="465">
-        <v>0.97795691541730323</v>
+        <f t="shared" si="3"/>
+        <v>0.97572073344607468</v>
       </c>
       <c r="R11" s="469">
         <v>2.204308458269677E-2</v>
@@ -46432,11 +46443,11 @@
         <v>0.57971648251948193</v>
       </c>
       <c r="T11" s="465">
-        <f t="shared" si="0"/>
-        <v>0.83357759339190229</v>
-      </c>
-    </row>
-    <row r="12" spans="1:21" s="89" customFormat="1" ht="13" hidden="1" x14ac:dyDescent="0.3">
+        <f t="shared" si="1"/>
+        <v>0.8316715470655488</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" s="89" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A12" s="268" t="s">
         <v>11</v>
       </c>
@@ -46485,8 +46496,9 @@
       <c r="P12" s="268">
         <v>1309</v>
       </c>
-      <c r="Q12" s="471">
-        <v>1.1906890072395</v>
+      <c r="Q12" s="465">
+        <f t="shared" si="3"/>
+        <v>1.1879663951802633</v>
       </c>
       <c r="R12" s="472" t="s">
         <v>563</v>
@@ -46496,8 +46508,8 @@
         <v>0.60840124055366307</v>
       </c>
       <c r="T12" s="465">
-        <f t="shared" si="0"/>
-        <v>1.0898060170991259</v>
+        <f t="shared" si="1"/>
+        <v>1.0873140826088075</v>
       </c>
     </row>
     <row r="13" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
@@ -46560,11 +46572,11 @@
         <v>0.55029781192188831</v>
       </c>
       <c r="T13" s="465">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.3270871954467218</v>
       </c>
     </row>
-    <row r="14" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" s="461" t="s">
         <v>11</v>
       </c>
@@ -46614,17 +46626,18 @@
         <v>1309</v>
       </c>
       <c r="Q14" s="465">
-        <v>0.87660484597724275</v>
+        <f t="shared" ref="Q14:Q16" si="4">M14/1312</f>
+        <v>0.87460041416479484</v>
       </c>
       <c r="R14" s="469">
         <v>0.12339515402275725</v>
       </c>
       <c r="T14" s="465">
-        <f t="shared" si="0"/>
-        <v>0.87660484597724275</v>
-      </c>
-    </row>
-    <row r="15" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>0.87460041416479484</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" s="461" t="s">
         <v>11</v>
       </c>
@@ -46674,7 +46687,8 @@
         <v>1309</v>
       </c>
       <c r="Q15" s="465">
-        <v>1.0379975404205701</v>
+        <f t="shared" si="4"/>
+        <v>1.0356240704348523</v>
       </c>
       <c r="R15" s="469" t="s">
         <v>563</v>
@@ -46684,11 +46698,11 @@
         <v>0.57396120733538203</v>
       </c>
       <c r="T15" s="465">
-        <f t="shared" si="0"/>
-        <v>1.0129943478066823</v>
-      </c>
-    </row>
-    <row r="16" spans="1:21" s="89" customFormat="1" ht="13" hidden="1" x14ac:dyDescent="0.3">
+        <f t="shared" si="1"/>
+        <v>1.0106780497552952</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" s="89" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A16" s="268" t="s">
         <v>11</v>
       </c>
@@ -46737,8 +46751,9 @@
       <c r="P16" s="268">
         <v>1309</v>
       </c>
-      <c r="Q16" s="471">
-        <v>1.2409943858609909</v>
+      <c r="Q16" s="465">
+        <f t="shared" si="4"/>
+        <v>1.2381567462591745</v>
       </c>
       <c r="R16" s="472" t="s">
         <v>563</v>
@@ -46748,11 +46763,11 @@
         <v>0.64793967587393286</v>
       </c>
       <c r="T16" s="465">
-        <f t="shared" si="0"/>
-        <v>1.2409943858609909</v>
-      </c>
-    </row>
-    <row r="17" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>1.2381567462591745</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="461" t="s">
         <v>11</v>
       </c>
@@ -46812,11 +46827,11 @@
         <v>0.68212128403389105</v>
       </c>
       <c r="T17" s="465">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.4520238319316896</v>
       </c>
     </row>
-    <row r="18" spans="1:20" s="468" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:21" s="468" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="466" t="s">
         <v>12</v>
       </c>
@@ -46866,18 +46881,20 @@
         <v>1309</v>
       </c>
       <c r="Q18" s="465">
-        <v>0.58823817163228931</v>
+        <f t="shared" ref="Q18:Q20" si="5">M18/1312</f>
+        <v>0.58689311483739837</v>
       </c>
       <c r="R18" s="469">
         <v>0.41176182836771069</v>
       </c>
       <c r="S18"/>
       <c r="T18" s="465">
-        <f t="shared" si="0"/>
-        <v>0.58823817163228931</v>
-      </c>
-    </row>
-    <row r="19" spans="1:20" s="468" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>0.58689311483739837</v>
+      </c>
+      <c r="U18" s="466"/>
+    </row>
+    <row r="19" spans="1:21" s="468" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="466" t="s">
         <v>12</v>
       </c>
@@ -46927,7 +46944,8 @@
         <v>1309</v>
       </c>
       <c r="Q19" s="465">
-        <v>0.79351760191508269</v>
+        <f t="shared" si="5"/>
+        <v>0.79170315617899634</v>
       </c>
       <c r="R19" s="469">
         <v>0.20648239808491731</v>
@@ -46937,11 +46955,15 @@
         <v>0.57634397849469465</v>
       </c>
       <c r="T19" s="465">
-        <f t="shared" si="0"/>
-        <v>0.58568868085574988</v>
-      </c>
-    </row>
-    <row r="20" spans="1:20" s="473" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+        <f t="shared" si="1"/>
+        <v>0.58434945368915903</v>
+      </c>
+      <c r="U19" s="466">
+        <f>100*(L19-L18)/E19</f>
+        <v>57.634397849469458</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" s="473" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A20" s="448" t="s">
         <v>12</v>
       </c>
@@ -46990,8 +47012,9 @@
       <c r="P20" s="461">
         <v>1309</v>
       </c>
-      <c r="Q20" s="474">
-        <v>1.0012409835299734</v>
+      <c r="Q20" s="465">
+        <f t="shared" si="5"/>
+        <v>0.99895156054934076</v>
       </c>
       <c r="R20" s="472" t="s">
         <v>563</v>
@@ -47001,11 +47024,11 @@
         <v>0.579774806006365</v>
       </c>
       <c r="T20" s="465">
-        <f t="shared" si="0"/>
-        <v>0.75746179384799073</v>
-      </c>
-    </row>
-    <row r="21" spans="1:20" s="468" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>0.75572979279498464</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" s="468" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="466" t="s">
         <v>12</v>
       </c>
@@ -47065,11 +47088,11 @@
         <v>0.59028877886608966</v>
       </c>
       <c r="T21" s="465">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.0685255920550039</v>
       </c>
     </row>
-    <row r="22" spans="1:20" s="468" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:21" s="468" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="466" t="s">
         <v>12</v>
       </c>
@@ -47119,18 +47142,20 @@
         <v>1309</v>
       </c>
       <c r="Q22" s="465">
-        <v>0.57902880909939725</v>
+        <f t="shared" ref="Q22:Q24" si="6">M22/1312</f>
+        <v>0.57770481029810294</v>
       </c>
       <c r="R22" s="469">
         <v>0.42097119090060275</v>
       </c>
       <c r="S22"/>
       <c r="T22" s="465">
-        <f t="shared" si="0"/>
-        <v>0.57902880909939725</v>
-      </c>
-    </row>
-    <row r="23" spans="1:20" s="468" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>0.57770481029810294</v>
+      </c>
+      <c r="U22" s="466"/>
+    </row>
+    <row r="23" spans="1:21" s="468" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="466" t="s">
         <v>12</v>
       </c>
@@ -47180,7 +47205,8 @@
         <v>1309</v>
       </c>
       <c r="Q23" s="465">
-        <v>0.75087735281385259</v>
+        <f t="shared" si="6"/>
+        <v>0.74916040764735747</v>
       </c>
       <c r="R23" s="469">
         <v>0.24912264718614741</v>
@@ -47190,11 +47216,15 @@
         <v>0.57897982226353006</v>
       </c>
       <c r="T23" s="465">
-        <f t="shared" si="0"/>
-        <v>0.57902880909939725</v>
-      </c>
-    </row>
-    <row r="24" spans="1:20" s="473" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+        <f t="shared" si="1"/>
+        <v>0.57770481029810283</v>
+      </c>
+      <c r="U23" s="466">
+        <f>100*(L23-L22)/E23</f>
+        <v>57.897982226353008</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" s="473" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A24" s="448" t="s">
         <v>12</v>
       </c>
@@ -47243,8 +47273,9 @@
       <c r="P24" s="461">
         <v>1309</v>
       </c>
-      <c r="Q24" s="471">
-        <v>0.92867385766270871</v>
+      <c r="Q24" s="465">
+        <f t="shared" si="6"/>
+        <v>0.92655036561012627</v>
       </c>
       <c r="R24" s="472">
         <v>7.1326142337291287E-2</v>
@@ -47254,11 +47285,11 @@
         <v>0.58899954488087114</v>
       </c>
       <c r="T24" s="465">
-        <f t="shared" si="0"/>
-        <v>0.68733087296276818</v>
-      </c>
-    </row>
-    <row r="25" spans="1:20" s="468" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>0.68575923224715218</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" s="468" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="466" t="s">
         <v>12</v>
       </c>
@@ -47318,11 +47349,11 @@
         <v>0.57911317532947271</v>
       </c>
       <c r="T25" s="465">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.89043799337916996</v>
       </c>
     </row>
-    <row r="26" spans="1:20" s="468" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:21" s="468" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="466" t="s">
         <v>12</v>
       </c>
@@ -47372,18 +47403,20 @@
         <v>1309</v>
       </c>
       <c r="Q26" s="465">
-        <v>0.60087986801265958</v>
+        <f t="shared" ref="Q26:Q28" si="7">M26/1312</f>
+        <v>0.59950590489982569</v>
       </c>
       <c r="R26" s="469">
         <v>0.39912013198734042</v>
       </c>
       <c r="S26"/>
       <c r="T26" s="465">
-        <f t="shared" si="0"/>
-        <v>0.60087986801265958</v>
-      </c>
-    </row>
-    <row r="27" spans="1:20" s="468" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>0.59950590489982569</v>
+      </c>
+      <c r="U26" s="466"/>
+    </row>
+    <row r="27" spans="1:21" s="468" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="466" t="s">
         <v>12</v>
       </c>
@@ -47433,7 +47466,8 @@
         <v>1309</v>
       </c>
       <c r="Q27" s="465">
-        <v>0.74675827708537934</v>
+        <f t="shared" si="7"/>
+        <v>0.74505075053716585</v>
       </c>
       <c r="R27" s="469">
         <v>0.25324172291462066</v>
@@ -47443,11 +47477,15 @@
         <v>0.57339695245585121</v>
       </c>
       <c r="T27" s="465">
-        <f t="shared" si="0"/>
-        <v>0.60087986801265947</v>
-      </c>
-    </row>
-    <row r="28" spans="1:20" s="473" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+        <f t="shared" si="1"/>
+        <v>0.59950590489982569</v>
+      </c>
+      <c r="U27" s="466">
+        <f>100*(L27-L26)/E27</f>
+        <v>57.339695245585126</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21" s="473" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A28" s="448" t="s">
         <v>12</v>
       </c>
@@ -47496,8 +47534,9 @@
       <c r="P28" s="461">
         <v>1309</v>
       </c>
-      <c r="Q28" s="471">
-        <v>0.90829861011401247</v>
+      <c r="Q28" s="465">
+        <f t="shared" si="7"/>
+        <v>0.90622170780430045</v>
       </c>
       <c r="R28" s="472">
         <v>9.1701389885987528E-2</v>
@@ -47507,11 +47546,11 @@
         <v>0.60417772228670097</v>
       </c>
       <c r="T28" s="465">
-        <f t="shared" si="0"/>
-        <v>0.68784937603856411</v>
-      </c>
-    </row>
-    <row r="29" spans="1:20" s="468" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>0.68627654972140262</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21" s="468" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="466" t="s">
         <v>12</v>
       </c>
@@ -47571,11 +47610,11 @@
         <v>0.54748213307724691</v>
       </c>
       <c r="T29" s="465">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.86863503573197032</v>
       </c>
     </row>
-    <row r="30" spans="1:20" s="468" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:21" s="468" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="466" t="s">
         <v>12</v>
       </c>
@@ -47625,18 +47664,20 @@
         <v>1309</v>
       </c>
       <c r="Q30" s="465">
-        <v>0.66789949509803936</v>
+        <f t="shared" ref="Q30:Q32" si="8">M30/1312</f>
+        <v>0.66637228588668718</v>
       </c>
       <c r="R30" s="469">
         <v>0.33210050490196064</v>
       </c>
       <c r="S30"/>
       <c r="T30" s="465">
-        <f t="shared" si="0"/>
-        <v>0.66789949509803936</v>
-      </c>
-    </row>
-    <row r="31" spans="1:20" s="468" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>0.66637228588668718</v>
+      </c>
+      <c r="U30" s="466"/>
+    </row>
+    <row r="31" spans="1:21" s="468" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="466" t="s">
         <v>12</v>
       </c>
@@ -47686,7 +47727,8 @@
         <v>1309</v>
       </c>
       <c r="Q31" s="465">
-        <v>0.79388603657372048</v>
+        <f t="shared" si="8"/>
+        <v>0.79207074838033542</v>
       </c>
       <c r="R31" s="469">
         <v>0.20611396342627952</v>
@@ -47696,11 +47738,15 @@
         <v>0.56595312604561276</v>
       </c>
       <c r="T31" s="465">
-        <f t="shared" si="0"/>
-        <v>0.66789949509803948</v>
-      </c>
-    </row>
-    <row r="32" spans="1:20" s="473" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+        <f t="shared" si="1"/>
+        <v>0.66637228588668729</v>
+      </c>
+      <c r="U31" s="466">
+        <f>100*(L31-L30)/E31</f>
+        <v>56.595312604561272</v>
+      </c>
+    </row>
+    <row r="32" spans="1:21" s="473" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A32" s="448" t="s">
         <v>12</v>
       </c>
@@ -47749,8 +47795,9 @@
       <c r="P32" s="461">
         <v>1309</v>
       </c>
-      <c r="Q32" s="471">
-        <v>0.9451237653726986</v>
+      <c r="Q32" s="465">
+        <f t="shared" si="8"/>
+        <v>0.94296265920187683</v>
       </c>
       <c r="R32" s="472">
         <v>5.4876234627301401E-2</v>
@@ -47760,11 +47807,11 @@
         <v>0.62266945556221442</v>
       </c>
       <c r="T32" s="465">
-        <f t="shared" si="0"/>
-        <v>0.79545017775810745</v>
-      </c>
-    </row>
-    <row r="33" spans="1:20" s="468" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>0.7936313130223801</v>
+      </c>
+    </row>
+    <row r="33" spans="1:21" s="468" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="466" t="s">
         <v>12</v>
       </c>
@@ -47824,11 +47871,11 @@
         <v>0.48984661022249432</v>
       </c>
       <c r="T33" s="465">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.93174304781872463</v>
       </c>
     </row>
-    <row r="34" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A34" s="461" t="s">
         <v>12</v>
       </c>
@@ -47878,17 +47925,18 @@
         <v>1309</v>
       </c>
       <c r="Q34" s="465">
-        <v>0.75746179384799073</v>
+        <f t="shared" ref="Q34:Q36" si="9">M34/1312</f>
+        <v>0.75572979279498464</v>
       </c>
       <c r="R34" s="469">
         <v>0.24253820615200927</v>
       </c>
       <c r="T34" s="465">
-        <f t="shared" si="0"/>
-        <v>0.75746179384799073</v>
-      </c>
-    </row>
-    <row r="35" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>0.75572979279498476</v>
+      </c>
+    </row>
+    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A35" s="461" t="s">
         <v>12</v>
       </c>
@@ -47938,7 +47986,8 @@
         <v>1309</v>
       </c>
       <c r="Q35" s="465">
-        <v>1.0685255920550039</v>
+        <f t="shared" si="9"/>
+        <v>1.0660823170731708</v>
       </c>
       <c r="R35" s="469" t="s">
         <v>563</v>
@@ -47948,48 +47997,52 @@
         <v>0.87334491710798634</v>
       </c>
       <c r="T35" s="465">
-        <f t="shared" si="0"/>
-        <v>1.0685255920550039</v>
-      </c>
-    </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A36" s="479" t="s">
+        <f t="shared" si="1"/>
+        <v>1.0660823170731708</v>
+      </c>
+      <c r="U35" s="466">
+        <f>100*(L35-L34)/E35</f>
+        <v>87.33449171079863</v>
+      </c>
+    </row>
+    <row r="36" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A36" s="478" t="s">
         <v>12</v>
       </c>
-      <c r="B36" s="479">
-        <v>0</v>
-      </c>
-      <c r="C36" s="479" t="s">
+      <c r="B36" s="478">
+        <v>0</v>
+      </c>
+      <c r="C36" s="478" t="s">
         <v>553</v>
       </c>
-      <c r="D36" s="478">
+      <c r="D36" s="477">
         <v>1</v>
       </c>
-      <c r="E36" s="479">
+      <c r="E36" s="478">
         <v>1398.7</v>
       </c>
-      <c r="F36" s="479">
+      <c r="F36" s="478">
         <v>1398.7</v>
       </c>
-      <c r="G36" s="479">
-        <v>0</v>
-      </c>
-      <c r="H36" s="479">
-        <v>0</v>
-      </c>
-      <c r="I36" s="479">
-        <v>0</v>
-      </c>
-      <c r="J36" s="479">
-        <v>0</v>
-      </c>
-      <c r="K36" s="479">
-        <v>0</v>
-      </c>
-      <c r="L36" s="479">
+      <c r="G36" s="478">
+        <v>0</v>
+      </c>
+      <c r="H36" s="478">
+        <v>0</v>
+      </c>
+      <c r="I36" s="478">
+        <v>0</v>
+      </c>
+      <c r="J36" s="478">
+        <v>0</v>
+      </c>
+      <c r="K36" s="478">
+        <v>0</v>
+      </c>
+      <c r="L36" s="478">
         <v>2797.4</v>
       </c>
-      <c r="M36" s="479">
+      <c r="M36" s="478">
         <v>1864.9333333333334</v>
       </c>
       <c r="N36" s="461">
@@ -48002,21 +48055,22 @@
         <v>1309</v>
       </c>
       <c r="Q36" s="465">
-        <v>1.4247007894066719</v>
+        <f t="shared" si="9"/>
+        <v>1.4214430894308943</v>
       </c>
       <c r="R36" s="469" t="s">
         <v>563</v>
       </c>
-      <c r="S36" s="478">
+      <c r="S36" s="477">
         <f>(L36-L34)/E36</f>
         <v>0.93667245855399306</v>
       </c>
       <c r="T36" s="465">
-        <f t="shared" si="0"/>
-        <v>1.4247007894066719</v>
-      </c>
-    </row>
-    <row r="37" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>1.4214430894308943</v>
+      </c>
+    </row>
+    <row r="37" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" s="461" t="s">
         <v>12</v>
       </c>
@@ -48076,11 +48130,11 @@
         <v>0.91676191122711348</v>
       </c>
       <c r="T37" s="465">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.7370453578154192</v>
       </c>
     </row>
-    <row r="38" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A38" s="461" t="s">
         <v>12</v>
       </c>
@@ -48130,17 +48184,18 @@
         <v>1309</v>
       </c>
       <c r="Q38" s="465">
-        <v>0.68733087296276818</v>
+        <f t="shared" ref="Q38:Q40" si="10">M38/1312</f>
+        <v>0.68575923224715218</v>
       </c>
       <c r="R38" s="469">
         <v>0.31266912703723182</v>
       </c>
       <c r="T38" s="465">
-        <f t="shared" si="0"/>
-        <v>0.68733087296276807</v>
-      </c>
-    </row>
-    <row r="39" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>0.68575923224715218</v>
+      </c>
+    </row>
+    <row r="39" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A39" s="461" t="s">
         <v>12</v>
       </c>
@@ -48190,7 +48245,8 @@
         <v>1309</v>
       </c>
       <c r="Q39" s="465">
-        <v>0.89043799337916996</v>
+        <f t="shared" si="10"/>
+        <v>0.88840193089430908</v>
       </c>
       <c r="R39" s="469">
         <v>0.10956200662083004</v>
@@ -48200,11 +48256,15 @@
         <v>0.68429398316311663</v>
       </c>
       <c r="T39" s="465">
-        <f t="shared" si="0"/>
-        <v>0.89043799337916996</v>
-      </c>
-    </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>0.88840193089430908</v>
+      </c>
+      <c r="U39" s="466">
+        <f>100*(L39-L38)/E39</f>
+        <v>68.429398316311662</v>
+      </c>
+    </row>
+    <row r="40" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A40" s="461" t="s">
         <v>12</v>
       </c>
@@ -48254,7 +48314,8 @@
         <v>1309</v>
       </c>
       <c r="Q40" s="465">
-        <v>1.1872506578388931</v>
+        <f t="shared" si="10"/>
+        <v>1.1845359078590785</v>
       </c>
       <c r="R40" s="469" t="s">
         <v>563</v>
@@ -48264,11 +48325,11 @@
         <v>0.84214699158155826</v>
       </c>
       <c r="T40" s="465">
-        <f t="shared" si="0"/>
-        <v>1.1872506578388931</v>
-      </c>
-    </row>
-    <row r="41" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>1.1845359078590785</v>
+      </c>
+    </row>
+    <row r="41" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" s="461" t="s">
         <v>12</v>
       </c>
@@ -48328,11 +48389,11 @@
         <v>0.89079029531512111</v>
       </c>
       <c r="T41" s="465">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.4805243960448029</v>
       </c>
     </row>
-    <row r="42" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A42" s="461" t="s">
         <v>12</v>
       </c>
@@ -48382,17 +48443,18 @@
         <v>1309</v>
       </c>
       <c r="Q42" s="465">
-        <v>0.687849376038564</v>
+        <f t="shared" ref="Q42:Q44" si="11">M42/1312</f>
+        <v>0.68627654972140262</v>
       </c>
       <c r="R42" s="469">
         <v>0.312150623961436</v>
       </c>
       <c r="T42" s="465">
-        <f t="shared" si="0"/>
-        <v>0.687849376038564</v>
-      </c>
-    </row>
-    <row r="43" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>0.68627654972140262</v>
+      </c>
+    </row>
+    <row r="43" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A43" s="461" t="s">
         <v>12</v>
       </c>
@@ -48442,7 +48504,8 @@
         <v>1309</v>
       </c>
       <c r="Q43" s="465">
-        <v>0.86863503573197032</v>
+        <f t="shared" si="11"/>
+        <v>0.86664882757099782</v>
       </c>
       <c r="R43" s="469">
         <v>0.13136496426802968</v>
@@ -48452,11 +48515,15 @@
         <v>0.7106051332397294</v>
       </c>
       <c r="T43" s="465">
-        <f t="shared" si="0"/>
-        <v>0.86863503573197043</v>
-      </c>
-    </row>
-    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>0.86664882757099793</v>
+      </c>
+      <c r="U43" s="466">
+        <f>100*(L43-L42)/E43</f>
+        <v>71.060513323972941</v>
+      </c>
+    </row>
+    <row r="44" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A44" s="461" t="s">
         <v>12</v>
       </c>
@@ -48506,7 +48573,8 @@
         <v>1309</v>
       </c>
       <c r="Q44" s="465">
-        <v>1.0842934589035613</v>
+        <f t="shared" si="11"/>
+        <v>1.0818141293481416</v>
       </c>
       <c r="R44" s="469" t="s">
         <v>563</v>
@@ -48516,11 +48584,11 @@
         <v>0.77914144519024175</v>
       </c>
       <c r="T44" s="465">
-        <f t="shared" si="0"/>
-        <v>1.0842934589035613</v>
-      </c>
-    </row>
-    <row r="45" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>1.0818141293481416</v>
+      </c>
+    </row>
+    <row r="45" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" s="461" t="s">
         <v>12</v>
       </c>
@@ -48580,11 +48648,11 @@
         <v>0.83622189471537423</v>
       </c>
       <c r="T45" s="465">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.3260811582814942</v>
       </c>
     </row>
-    <row r="46" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A46" s="461" t="s">
         <v>12</v>
       </c>
@@ -48634,17 +48702,18 @@
         <v>1309</v>
       </c>
       <c r="Q46" s="465">
-        <v>0.79545017775810756</v>
+        <f t="shared" ref="Q46:Q48" si="12">M46/1312</f>
+        <v>0.79363131302238021</v>
       </c>
       <c r="R46" s="469">
         <v>0.20454982224189244</v>
       </c>
       <c r="T46" s="465">
-        <f t="shared" si="0"/>
-        <v>0.79545017775810756</v>
-      </c>
-    </row>
-    <row r="47" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>0.79363131302238021</v>
+      </c>
+    </row>
+    <row r="47" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A47" s="461" t="s">
         <v>12</v>
       </c>
@@ -48694,7 +48763,8 @@
         <v>1309</v>
       </c>
       <c r="Q47" s="465">
-        <v>0.93174304781872463</v>
+        <f t="shared" si="12"/>
+        <v>0.92961253780084641</v>
       </c>
       <c r="R47" s="469">
         <v>6.8256952181275365E-2</v>
@@ -48704,11 +48774,15 @@
         <v>0.61225091954305388</v>
       </c>
       <c r="T47" s="465">
-        <f t="shared" si="0"/>
-        <v>0.93174304781872463</v>
-      </c>
-    </row>
-    <row r="48" spans="1:20" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>0.92961253780084641</v>
+      </c>
+      <c r="U47" s="466">
+        <f>100*(L47-L46)/E47</f>
+        <v>61.225091954305384</v>
+      </c>
+    </row>
+    <row r="48" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A48" s="461" t="s">
         <v>12</v>
       </c>
@@ -48758,7 +48832,8 @@
         <v>1309</v>
       </c>
       <c r="Q48" s="465">
-        <v>1.098808025958028</v>
+        <f t="shared" si="12"/>
+        <v>1.0962955076059897</v>
       </c>
       <c r="R48" s="469" t="s">
         <v>563</v>
@@ -48768,11 +48843,11 @@
         <v>0.68136770994843066</v>
       </c>
       <c r="T48" s="465">
-        <f t="shared" si="0"/>
-        <v>1.098808025958028</v>
-      </c>
-    </row>
-    <row r="49" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>1.0962955076059897</v>
+      </c>
+    </row>
+    <row r="49" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" s="461" t="s">
         <v>12</v>
       </c>
@@ -48832,11 +48907,11 @@
         <v>0.76226157651873361</v>
       </c>
       <c r="T49" s="465">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.3045101792271454</v>
       </c>
     </row>
-    <row r="50" spans="1:20" s="468" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:21" s="468" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="466" t="s">
         <v>12</v>
       </c>
@@ -48886,18 +48961,19 @@
         <v>1309</v>
       </c>
       <c r="Q50" s="465">
-        <v>1.0012409835299734</v>
+        <f t="shared" ref="Q50:Q52" si="13">M50/1312</f>
+        <v>0.99895156054934076</v>
       </c>
       <c r="R50" s="469" t="s">
         <v>563</v>
       </c>
       <c r="S50"/>
       <c r="T50" s="465">
-        <f t="shared" si="0"/>
-        <v>0.75746179384799073</v>
-      </c>
-    </row>
-    <row r="51" spans="1:20" s="468" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>0.75572979279498464</v>
+      </c>
+    </row>
+    <row r="51" spans="1:21" s="468" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="466" t="s">
         <v>12</v>
       </c>
@@ -48947,7 +49023,8 @@
         <v>1309</v>
       </c>
       <c r="Q51" s="465">
-        <v>1.2189768385536031</v>
+        <f t="shared" si="13"/>
+        <v>1.216189543953252</v>
       </c>
       <c r="R51" s="469" t="s">
         <v>563</v>
@@ -48957,11 +49034,15 @@
         <v>0.61131672458553921</v>
       </c>
       <c r="T51" s="465">
-        <f t="shared" si="0"/>
-        <v>1.0685255920550039</v>
-      </c>
-    </row>
-    <row r="52" spans="1:20" s="473" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+        <f t="shared" si="1"/>
+        <v>1.0660823170731708</v>
+      </c>
+      <c r="U51" s="466">
+        <f>100*(L51-L50)/E51</f>
+        <v>61.131672458553915</v>
+      </c>
+    </row>
+    <row r="52" spans="1:21" s="473" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A52" s="448" t="s">
         <v>12</v>
       </c>
@@ -49010,8 +49091,9 @@
       <c r="P52" s="461">
         <v>1309</v>
       </c>
-      <c r="Q52" s="471">
-        <v>1.5287559485612428</v>
+      <c r="Q52" s="465">
+        <f t="shared" si="13"/>
+        <v>1.5252603175813009</v>
       </c>
       <c r="R52" s="472" t="s">
         <v>563</v>
@@ -49021,11 +49103,11 @@
         <v>0.74052737101515487</v>
       </c>
       <c r="T52" s="465">
-        <f t="shared" si="0"/>
-        <v>1.4247007894066717</v>
-      </c>
-    </row>
-    <row r="53" spans="1:20" s="468" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>1.4214430894308943</v>
+      </c>
+    </row>
+    <row r="53" spans="1:21" s="468" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" s="466" t="s">
         <v>12</v>
       </c>
@@ -49085,11 +49167,11 @@
         <v>0.68861651958221803</v>
       </c>
       <c r="T53" s="465">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.7370453578154192</v>
       </c>
     </row>
-    <row r="54" spans="1:20" s="468" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:21" s="468" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="466" t="s">
         <v>12</v>
       </c>
@@ -49139,18 +49221,19 @@
         <v>1309</v>
       </c>
       <c r="Q54" s="465">
-        <v>0.92867385766270871</v>
+        <f t="shared" ref="Q54:Q56" si="14">M54/1312</f>
+        <v>0.92655036561012627</v>
       </c>
       <c r="R54" s="469">
         <v>7.1326142337291287E-2</v>
       </c>
       <c r="S54"/>
       <c r="T54" s="465">
-        <f t="shared" si="0"/>
-        <v>0.68733087296276818</v>
-      </c>
-    </row>
-    <row r="55" spans="1:20" s="468" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>0.68575923224715218</v>
+      </c>
+    </row>
+    <row r="55" spans="1:21" s="468" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="466" t="s">
         <v>12</v>
       </c>
@@ -49200,7 +49283,8 @@
         <v>1309</v>
       </c>
       <c r="Q55" s="465">
-        <v>1.0946931828792124</v>
+        <f t="shared" si="14"/>
+        <v>1.092190073467141</v>
       </c>
       <c r="R55" s="469" t="s">
         <v>563</v>
@@ -49210,11 +49294,15 @@
         <v>0.55934043622667584</v>
       </c>
       <c r="T55" s="465">
-        <f t="shared" si="0"/>
-        <v>0.89043799337916996</v>
-      </c>
-    </row>
-    <row r="56" spans="1:20" s="473" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+        <f t="shared" si="1"/>
+        <v>0.88840193089430908</v>
+      </c>
+      <c r="U55" s="466">
+        <f>100*(L55-L54)/E55</f>
+        <v>55.934043622667595</v>
+      </c>
+    </row>
+    <row r="56" spans="1:21" s="473" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A56" s="448" t="s">
         <v>12</v>
       </c>
@@ -49263,8 +49351,9 @@
       <c r="P56" s="461">
         <v>1309</v>
       </c>
-      <c r="Q56" s="471">
-        <v>1.3528424412189117</v>
+      <c r="Q56" s="465">
+        <f t="shared" si="14"/>
+        <v>1.3497490514905148</v>
       </c>
       <c r="R56" s="472" t="s">
         <v>563</v>
@@ -49274,11 +49363,11 @@
         <v>0.71453922683572291</v>
       </c>
       <c r="T56" s="465">
-        <f t="shared" si="0"/>
-        <v>1.1872506578388928</v>
-      </c>
-    </row>
-    <row r="57" spans="1:20" s="468" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>1.1845359078590785</v>
+      </c>
+    </row>
+    <row r="57" spans="1:21" s="468" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" s="466" t="s">
         <v>12</v>
       </c>
@@ -49338,11 +49427,11 @@
         <v>0.67636845215123109</v>
       </c>
       <c r="T57" s="465">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.4805243960448027</v>
       </c>
     </row>
-    <row r="58" spans="1:20" s="468" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:21" s="468" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="466" t="s">
         <v>12</v>
       </c>
@@ -49392,18 +49481,19 @@
         <v>1309</v>
       </c>
       <c r="Q58" s="465">
-        <v>0.90829861011401247</v>
+        <f t="shared" ref="Q58:Q60" si="15">M58/1312</f>
+        <v>0.90622170780430045</v>
       </c>
       <c r="R58" s="469">
         <v>9.1701389885987528E-2</v>
       </c>
       <c r="S58"/>
       <c r="T58" s="465">
-        <f t="shared" si="0"/>
-        <v>0.68784937603856411</v>
-      </c>
-    </row>
-    <row r="59" spans="1:20" s="468" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>0.68627654972140262</v>
+      </c>
+    </row>
+    <row r="59" spans="1:21" s="468" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="466" t="s">
         <v>12</v>
       </c>
@@ -49453,7 +49543,8 @@
         <v>1309</v>
       </c>
       <c r="Q59" s="465">
-        <v>1.0187360611454466</v>
+        <f t="shared" si="15"/>
+        <v>1.016406634176364</v>
       </c>
       <c r="R59" s="469" t="s">
         <v>563</v>
@@ -49463,11 +49554,15 @@
         <v>0.43409095465833875</v>
       </c>
       <c r="T59" s="465">
-        <f t="shared" si="0"/>
-        <v>0.86863503573197032</v>
-      </c>
-    </row>
-    <row r="60" spans="1:20" s="473" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+        <f t="shared" si="1"/>
+        <v>0.86664882757099782</v>
+      </c>
+      <c r="U59" s="466">
+        <f>100*(L59-L58)/E59</f>
+        <v>43.409095465833872</v>
+      </c>
+    </row>
+    <row r="60" spans="1:21" s="473" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A60" s="448" t="s">
         <v>12</v>
       </c>
@@ -49516,8 +49611,9 @@
       <c r="P60" s="461">
         <v>1309</v>
       </c>
-      <c r="Q60" s="471">
-        <v>1.239813091847648</v>
+      <c r="Q60" s="465">
+        <f t="shared" si="15"/>
+        <v>1.2369781533754354</v>
       </c>
       <c r="R60" s="472" t="s">
         <v>563</v>
@@ -49527,11 +49623,11 @@
         <v>0.65153368044440618</v>
       </c>
       <c r="T60" s="465">
-        <f t="shared" si="0"/>
-        <v>1.0842934589035613</v>
-      </c>
-    </row>
-    <row r="61" spans="1:20" s="468" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>1.0818141293481418</v>
+      </c>
+    </row>
+    <row r="61" spans="1:21" s="468" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" s="466" t="s">
         <v>12</v>
       </c>
@@ -49591,11 +49687,11 @@
         <v>0.6218000515514841</v>
       </c>
       <c r="T61" s="465">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.3260811582814942</v>
       </c>
     </row>
-    <row r="62" spans="1:20" s="468" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:21" s="468" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="466" t="s">
         <v>12</v>
       </c>
@@ -49645,18 +49741,19 @@
         <v>1309</v>
       </c>
       <c r="Q62" s="465">
-        <v>0.9451237653726986</v>
+        <f t="shared" ref="Q62:Q64" si="16">M62/1312</f>
+        <v>0.94296265920187683</v>
       </c>
       <c r="R62" s="469">
         <v>5.4876234627301401E-2</v>
       </c>
       <c r="S62"/>
       <c r="T62" s="465">
-        <f t="shared" si="0"/>
-        <v>0.79545017775810745</v>
-      </c>
-    </row>
-    <row r="63" spans="1:20" s="468" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>0.7936313130223801</v>
+      </c>
+    </row>
+    <row r="63" spans="1:21" s="468" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="466" t="s">
         <v>12</v>
       </c>
@@ -49706,7 +49803,8 @@
         <v>1309</v>
       </c>
       <c r="Q63" s="465">
-        <v>1.0258051276793054</v>
+        <f t="shared" si="16"/>
+        <v>1.0234595366861363</v>
       </c>
       <c r="R63" s="469" t="s">
         <v>563</v>
@@ -49716,48 +49814,52 @@
         <v>0.36243450035380781</v>
       </c>
       <c r="T63" s="465">
-        <f t="shared" si="0"/>
-        <v>0.96251515589741077</v>
-      </c>
-    </row>
-    <row r="64" spans="1:20" s="473" customFormat="1" ht="13" x14ac:dyDescent="0.3">
-      <c r="A64" s="476" t="s">
+        <f t="shared" si="1"/>
+        <v>0.96031428282752351</v>
+      </c>
+      <c r="U63" s="466">
+        <f>100*(L63-L62)/E63</f>
+        <v>36.243450035380782</v>
+      </c>
+    </row>
+    <row r="64" spans="1:21" s="473" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+      <c r="A64" s="475" t="s">
         <v>12</v>
       </c>
-      <c r="B64" s="476">
+      <c r="B64" s="475">
         <v>3</v>
       </c>
-      <c r="C64" s="476" t="s">
+      <c r="C64" s="475" t="s">
         <v>554</v>
       </c>
-      <c r="D64" s="477">
+      <c r="D64" s="476">
         <v>1</v>
       </c>
-      <c r="E64" s="476">
+      <c r="E64" s="475">
         <v>1398.7</v>
       </c>
-      <c r="F64" s="476">
+      <c r="F64" s="475">
         <v>1398.7</v>
       </c>
-      <c r="G64" s="476">
+      <c r="G64" s="475">
         <v>601.49917905999996</v>
       </c>
-      <c r="H64" s="476">
+      <c r="H64" s="475">
         <v>53.116115289740293</v>
       </c>
-      <c r="I64" s="476">
-        <v>0</v>
-      </c>
-      <c r="J64" s="476">
+      <c r="I64" s="475">
+        <v>0</v>
+      </c>
+      <c r="J64" s="475">
         <v>238.87902758670813</v>
       </c>
-      <c r="K64" s="476">
-        <v>0</v>
-      </c>
-      <c r="L64" s="476">
+      <c r="K64" s="475">
+        <v>0</v>
+      </c>
+      <c r="L64" s="475">
         <v>3690.8943219364483</v>
       </c>
-      <c r="M64" s="476">
+      <c r="M64" s="475">
         <v>1537.8726341401868</v>
       </c>
       <c r="N64" s="448">
@@ -49769,22 +49871,23 @@
       <c r="P64" s="461">
         <v>1309</v>
       </c>
-      <c r="Q64" s="471">
-        <v>1.174845404232381</v>
+      <c r="Q64" s="465">
+        <f t="shared" si="16"/>
+        <v>1.1721590199239229</v>
       </c>
       <c r="R64" s="472" t="s">
         <v>563</v>
       </c>
-      <c r="S64" s="478">
+      <c r="S64" s="477">
         <f>(L64-L62)/E64</f>
         <v>0.51597447675811703</v>
       </c>
       <c r="T64" s="465">
-        <f t="shared" si="0"/>
-        <v>1.0988080259580277</v>
-      </c>
-    </row>
-    <row r="65" spans="1:20" s="468" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>1.0962955076059897</v>
+      </c>
+    </row>
+    <row r="65" spans="1:21" s="468" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" s="466" t="s">
         <v>12</v>
       </c>
@@ -49844,11 +49947,11 @@
         <v>0.54783973335484359</v>
       </c>
       <c r="T65" s="465">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.3045101792271454</v>
       </c>
     </row>
-    <row r="66" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A66" s="461" t="s">
         <v>12</v>
       </c>
@@ -49898,17 +50001,18 @@
         <v>1309</v>
       </c>
       <c r="Q66" s="465">
-        <v>1.2189768385536031</v>
+        <f t="shared" ref="Q66:Q68" si="17">M66/1312</f>
+        <v>1.216189543953252</v>
       </c>
       <c r="R66" s="469" t="s">
         <v>563</v>
       </c>
       <c r="T66" s="465">
-        <f t="shared" si="0"/>
-        <v>1.0685255920550039</v>
-      </c>
-    </row>
-    <row r="67" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>1.0660823170731708</v>
+      </c>
+    </row>
+    <row r="67" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A67" s="461" t="s">
         <v>12</v>
       </c>
@@ -49958,7 +50062,8 @@
         <v>1309</v>
       </c>
       <c r="Q67" s="465">
-        <v>1.4369382505729562</v>
+        <f t="shared" si="17"/>
+        <v>1.4336525685975607</v>
       </c>
       <c r="R67" s="469" t="s">
         <v>563</v>
@@ -49968,11 +50073,15 @@
         <v>0.61195000000000022</v>
       </c>
       <c r="T67" s="465">
-        <f t="shared" ref="T67:T81" si="1">(L67-J67)*Q67/L67</f>
-        <v>1.4247007894066717</v>
-      </c>
-    </row>
-    <row r="68" spans="1:20" x14ac:dyDescent="0.25">
+        <f t="shared" ref="T67:T81" si="18">(L67-J67)*Q67/L67</f>
+        <v>1.4214430894308943</v>
+      </c>
+      <c r="U67" s="466">
+        <f>100*(L67-L66)/E67</f>
+        <v>61.195000000000014</v>
+      </c>
+    </row>
+    <row r="68" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A68" s="461" t="s">
         <v>12</v>
       </c>
@@ -50022,7 +50131,8 @@
         <v>1309</v>
       </c>
       <c r="Q68" s="465">
-        <v>1.7370453578154192</v>
+        <f t="shared" si="17"/>
+        <v>1.7330734553204143</v>
       </c>
       <c r="R68" s="469" t="s">
         <v>563</v>
@@ -50032,11 +50142,11 @@
         <v>0.7272664170805575</v>
       </c>
       <c r="T68" s="465">
-        <f t="shared" si="1"/>
-        <v>1.7370453578154192</v>
-      </c>
-    </row>
-    <row r="69" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+        <f t="shared" si="18"/>
+        <v>1.7330734553204141</v>
+      </c>
+    </row>
+    <row r="69" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" s="461" t="s">
         <v>12</v>
       </c>
@@ -50096,11 +50206,11 @@
         <v>0.76848016339498626</v>
       </c>
       <c r="T69" s="465">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>2.040117560127757</v>
       </c>
     </row>
-    <row r="70" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A70" s="461" t="s">
         <v>12</v>
       </c>
@@ -50150,17 +50260,18 @@
         <v>1309</v>
       </c>
       <c r="Q70" s="465">
-        <v>1.0946931828792124</v>
+        <f t="shared" ref="Q70:Q72" si="19">M70/1312</f>
+        <v>1.092190073467141</v>
       </c>
       <c r="R70" s="469" t="s">
         <v>563</v>
       </c>
       <c r="T70" s="465">
-        <f t="shared" si="1"/>
-        <v>0.89043799337916996</v>
-      </c>
-    </row>
-    <row r="71" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+        <f t="shared" si="18"/>
+        <v>0.88840193089430908</v>
+      </c>
+    </row>
+    <row r="71" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A71" s="461" t="s">
         <v>12</v>
       </c>
@@ -50210,7 +50321,8 @@
         <v>1309</v>
       </c>
       <c r="Q71" s="465">
-        <v>1.2763276928953398</v>
+        <f t="shared" si="19"/>
+        <v>1.2734092606707317</v>
       </c>
       <c r="R71" s="469" t="s">
         <v>563</v>
@@ -50220,11 +50332,15 @@
         <v>0.61194999999999955</v>
       </c>
       <c r="T71" s="465">
-        <f t="shared" si="1"/>
-        <v>1.1872506578388931</v>
-      </c>
-    </row>
-    <row r="72" spans="1:20" x14ac:dyDescent="0.25">
+        <f t="shared" si="18"/>
+        <v>1.1845359078590787</v>
+      </c>
+      <c r="U71" s="466">
+        <f>100*(L71-L70)/E71</f>
+        <v>61.194999999999951</v>
+      </c>
+    </row>
+    <row r="72" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A72" s="461" t="s">
         <v>12</v>
       </c>
@@ -50274,7 +50390,8 @@
         <v>1309</v>
       </c>
       <c r="Q72" s="465">
-        <v>1.5309380249812259</v>
+        <f t="shared" si="19"/>
+        <v>1.5274374044972749</v>
       </c>
       <c r="R72" s="469" t="s">
         <v>563</v>
@@ -50284,11 +50401,11 @@
         <v>0.73488246011350866</v>
       </c>
       <c r="T72" s="465">
-        <f t="shared" si="1"/>
-        <v>1.4805243960448027</v>
-      </c>
-    </row>
-    <row r="73" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+        <f t="shared" si="18"/>
+        <v>1.4771390506270172</v>
+      </c>
+    </row>
+    <row r="73" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" s="461" t="s">
         <v>12</v>
       </c>
@@ -50348,11 +50465,11 @@
         <v>0.71694086113345235</v>
       </c>
       <c r="T73" s="465">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>1.7330845646384176</v>
       </c>
     </row>
-    <row r="74" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A74" s="461" t="s">
         <v>12</v>
       </c>
@@ -50402,17 +50519,18 @@
         <v>1309</v>
       </c>
       <c r="Q74" s="465">
-        <v>1.0187360611454466</v>
+        <f t="shared" ref="Q74:Q76" si="20">M74/1312</f>
+        <v>1.016406634176364</v>
       </c>
       <c r="R74" s="469" t="s">
         <v>563</v>
       </c>
       <c r="T74" s="465">
-        <f t="shared" si="1"/>
-        <v>0.86863503573197032</v>
-      </c>
-    </row>
-    <row r="75" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+        <f t="shared" si="18"/>
+        <v>0.86664882757099782</v>
+      </c>
+    </row>
+    <row r="75" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A75" s="461" t="s">
         <v>12</v>
       </c>
@@ -50462,7 +50580,8 @@
         <v>1309</v>
       </c>
       <c r="Q75" s="465">
-        <v>1.1742290218560152</v>
+        <f t="shared" si="20"/>
+        <v>1.1715440469584786</v>
       </c>
       <c r="R75" s="469" t="s">
         <v>563</v>
@@ -50472,11 +50591,15 @@
         <v>0.61118838878570392</v>
       </c>
       <c r="T75" s="465">
-        <f t="shared" si="1"/>
-        <v>1.0842934589035615</v>
-      </c>
-    </row>
-    <row r="76" spans="1:20" x14ac:dyDescent="0.25">
+        <f t="shared" si="18"/>
+        <v>1.0818141293481418</v>
+      </c>
+      <c r="U75" s="466">
+        <f>100*(L75-L74)/E75</f>
+        <v>61.118838878570386</v>
+      </c>
+    </row>
+    <row r="76" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A76" s="461" t="s">
         <v>12</v>
       </c>
@@ -50526,7 +50649,8 @@
         <v>1309</v>
       </c>
       <c r="Q76" s="465">
-        <v>1.3828766588453563</v>
+        <f t="shared" si="20"/>
+        <v>1.3797145933144599</v>
       </c>
       <c r="R76" s="469" t="s">
         <v>563</v>
@@ -50536,11 +50660,11 @@
         <v>0.71565459999805692</v>
       </c>
       <c r="T76" s="465">
-        <f t="shared" si="1"/>
-        <v>1.3260811582814942</v>
-      </c>
-    </row>
-    <row r="77" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+        <f t="shared" si="18"/>
+        <v>1.3230489605110334</v>
+      </c>
+    </row>
+    <row r="77" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" s="461" t="s">
         <v>12</v>
       </c>
@@ -50600,11 +50724,11 @@
         <v>0.71939553900455699</v>
       </c>
       <c r="T77" s="465">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>1.5678021641715698</v>
       </c>
     </row>
-    <row r="78" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A78" s="461" t="s">
         <v>12</v>
       </c>
@@ -50654,17 +50778,18 @@
         <v>1309</v>
       </c>
       <c r="Q78" s="465">
-        <v>0.99503301960061907</v>
+        <f t="shared" ref="Q78:Q80" si="21">M78/1312</f>
+        <v>0.9927577916594591</v>
       </c>
       <c r="R78" s="469">
         <v>4.9669803993809269E-3</v>
       </c>
       <c r="T78" s="465">
-        <f t="shared" si="1"/>
-        <v>0.93174304781872463</v>
-      </c>
-    </row>
-    <row r="79" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+        <f t="shared" si="18"/>
+        <v>0.92961253780084641</v>
+      </c>
+    </row>
+    <row r="79" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A79" s="461" t="s">
         <v>12</v>
       </c>
@@ -50714,7 +50839,8 @@
         <v>1309</v>
       </c>
       <c r="Q79" s="465">
-        <v>1.1174593429897024</v>
+        <f t="shared" si="21"/>
+        <v>1.1149041768090857</v>
       </c>
       <c r="R79" s="469" t="s">
         <v>563</v>
@@ -50724,11 +50850,15 @@
         <v>0.54996001652841076</v>
       </c>
       <c r="T79" s="465">
-        <f t="shared" si="1"/>
-        <v>1.098808025958028</v>
-      </c>
-    </row>
-    <row r="80" spans="1:20" x14ac:dyDescent="0.25">
+        <f t="shared" si="18"/>
+        <v>1.0962955076059899</v>
+      </c>
+      <c r="U79" s="466">
+        <f>100*(L79-L78)/E79</f>
+        <v>54.996001652841073</v>
+      </c>
+    </row>
+    <row r="80" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A80" s="461" t="s">
         <v>12</v>
       </c>
@@ -50778,7 +50908,8 @@
         <v>1309</v>
       </c>
       <c r="Q80" s="465">
-        <v>1.3109867500190986</v>
+        <f t="shared" si="21"/>
+        <v>1.3079890669016767</v>
       </c>
       <c r="R80" s="469" t="s">
         <v>563</v>
@@ -50788,8 +50919,8 @@
         <v>0.70965914026073829</v>
       </c>
       <c r="T80" s="465">
-        <f t="shared" si="1"/>
-        <v>1.3045101792271454</v>
+        <f t="shared" si="18"/>
+        <v>1.3015273053417173</v>
       </c>
     </row>
     <row r="81" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
@@ -50852,20 +50983,17 @@
         <v>0.76366333420209043</v>
       </c>
       <c r="T81" s="465">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>1.505029154793736</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:U81" xr:uid="{06BA5670-E00D-4C7C-B258-F1FFD02B92CB}">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="couple"/>
-      </filters>
-    </filterColumn>
     <filterColumn colId="4">
       <filters>
+        <filter val="0"/>
         <filter val="1399"/>
+        <filter val="699"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>